<commit_message>
add ip['qrr_vs_i'], new cyntec inductors
</commit_message>
<xml_diff>
--- a/data/cyntec_inductor_data.xlsx
+++ b/data/cyntec_inductor_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://renesasgroup-my.sharepoint.com/personal/gary_kidwell_wz_renesas_com/Documents/python/charger/mathmodels/pdis_2or3lvl_bb/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="676" documentId="11_88A5EEC595FCDE19E65C93C75DD0486FD8C93E14" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C71671D6-CD4D-4CB0-84FB-6976FEBA916E}"/>
+  <xr:revisionPtr revIDLastSave="803" documentId="11_88A5EEC595FCDE19E65C93C75DD0486FD8C93E14" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{160B5F0C-4B7F-4577-AABA-9F5AB12CA9CB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16260" tabRatio="772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="772" firstSheet="11" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="htel20121b" sheetId="21" r:id="rId1"/>
@@ -31,7 +31,13 @@
     <sheet name="hbed063t" sheetId="18" r:id="rId16"/>
     <sheet name="cmll063t" sheetId="17" r:id="rId17"/>
     <sheet name="pimb063t" sheetId="11" r:id="rId18"/>
-    <sheet name="cmlb104t" sheetId="4" r:id="rId19"/>
+    <sheet name="cmle064t" sheetId="24" r:id="rId19"/>
+    <sheet name="cmle083t" sheetId="27" r:id="rId20"/>
+    <sheet name="cmle103t" sheetId="25" r:id="rId21"/>
+    <sheet name="cmle104t" sheetId="26" r:id="rId22"/>
+    <sheet name="cmlb104t" sheetId="4" r:id="rId23"/>
+    <sheet name="cmle105t" sheetId="28" r:id="rId24"/>
+    <sheet name="cmls135t" sheetId="23" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="39">
   <si>
     <t>Lout</t>
   </si>
@@ -151,6 +157,24 @@
   <si>
     <t>htel20121b</t>
   </si>
+  <si>
+    <t>cmls135t</t>
+  </si>
+  <si>
+    <t>cmle064t</t>
+  </si>
+  <si>
+    <t>cmle103t</t>
+  </si>
+  <si>
+    <t>cmle104t</t>
+  </si>
+  <si>
+    <t>cmle083t</t>
+  </si>
+  <si>
+    <t>cmle105t</t>
+  </si>
 </sst>
 </file>
 
@@ -193,12 +217,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1396,7 +1421,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:N5"/>
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2260,7 +2285,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2518,746 +2543,102 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04542642-2AB9-4E4E-BC92-700C7AD35014}">
-  <dimension ref="A1:N16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1BC573D-AEF5-48A1-9870-479DF8E5F424}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0.36</v>
+        <v>0.42</v>
       </c>
       <c r="B2">
-        <v>1.0499999999999999E-3</v>
+        <v>1.5499999999999999E-3</v>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>51</v>
-      </c>
-      <c r="E2" s="2">
+        <v>23</v>
+      </c>
+      <c r="E2">
         <f>40/F2</f>
-        <v>30.419002751018571</v>
-      </c>
-      <c r="F2" s="1">
+        <v>38.959015116097873</v>
+      </c>
+      <c r="F2">
         <f>C2^2*B2*1.15</f>
-        <v>1.3149674999999996</v>
-      </c>
-      <c r="G2">
-        <v>4.4962287207989402E-3</v>
+        <v>1.0267199999999999</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.7699999999999999E-4</v>
       </c>
       <c r="H2">
-        <v>2.7906976744186043E-3</v>
+        <v>5.8300000000000001E-3</v>
       </c>
       <c r="I2">
-        <v>1.0280380382624399</v>
+        <v>1.101</v>
       </c>
       <c r="J2">
-        <v>2.51785650480713</v>
+        <v>2.2490000000000001</v>
       </c>
       <c r="K2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="L2">
-        <v>13.6</v>
+        <v>8.4</v>
       </c>
       <c r="M2">
-        <v>10.3</v>
+        <v>6.8</v>
       </c>
       <c r="N2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>0.47</v>
-      </c>
-      <c r="B3">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="C3">
-        <v>32</v>
-      </c>
-      <c r="D3">
-        <v>46</v>
-      </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E16" si="0">40/F3</f>
-        <v>26.128762541806022</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F16" si="1">C3^2*B3*1.15</f>
-        <v>1.5308799999999998</v>
-      </c>
-      <c r="G3">
-        <v>4.0935840852075502E-3</v>
-      </c>
-      <c r="H3">
-        <v>3.5619552860932172E-3</v>
-      </c>
-      <c r="I3">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J3">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3">
-        <v>13.6</v>
-      </c>
-      <c r="M3">
-        <v>10.3</v>
-      </c>
-      <c r="N3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="B4">
-        <v>1.5900000000000001E-3</v>
-      </c>
-      <c r="C4">
-        <v>25</v>
-      </c>
-      <c r="D4">
-        <v>33.5</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" si="0"/>
-        <v>35.001367240907847</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" si="1"/>
-        <v>1.1428125</v>
-      </c>
-      <c r="G4">
-        <v>4.50692554059053E-3</v>
-      </c>
-      <c r="H4">
-        <v>3.695150115473441E-3</v>
-      </c>
-      <c r="I4">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J4">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4">
-        <v>13.6</v>
-      </c>
-      <c r="M4">
-        <v>10.3</v>
-      </c>
-      <c r="N4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>2.8500000000000001E-3</v>
-      </c>
-      <c r="C5">
-        <v>19</v>
-      </c>
-      <c r="D5">
-        <v>29</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="0"/>
-        <v>33.807268985422731</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="1"/>
-        <v>1.1831775</v>
-      </c>
-      <c r="G5">
-        <v>4.2248688117616879E-3</v>
-      </c>
-      <c r="H5">
-        <v>5.4815545688757326E-3</v>
-      </c>
-      <c r="I5">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J5">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5">
-        <v>13.6</v>
-      </c>
-      <c r="M5">
-        <v>10.3</v>
-      </c>
-      <c r="N5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1.5</v>
-      </c>
-      <c r="B6">
-        <v>3.8E-3</v>
-      </c>
-      <c r="C6">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>35.755148741418765</v>
-      </c>
-      <c r="F6" s="1">
-        <f t="shared" si="1"/>
-        <v>1.1187199999999999</v>
-      </c>
-      <c r="G6">
-        <v>3.9161453990648959E-3</v>
-      </c>
-      <c r="H6">
-        <v>6.4811614241272048E-3</v>
-      </c>
-      <c r="I6">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J6">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K6" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6">
-        <v>13.6</v>
-      </c>
-      <c r="M6">
-        <v>10.3</v>
-      </c>
-      <c r="N6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B7">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>20</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>40.257648953301128</v>
-      </c>
-      <c r="F7" s="1">
-        <f t="shared" si="1"/>
-        <v>0.99359999999999993</v>
-      </c>
-      <c r="G7">
-        <v>3.9723160813784969E-3</v>
-      </c>
-      <c r="H7">
-        <v>8.175399479747306E-3</v>
-      </c>
-      <c r="I7">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J7">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7">
-        <v>13.6</v>
-      </c>
-      <c r="M7">
-        <v>10.3</v>
-      </c>
-      <c r="N7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>3.3</v>
-      </c>
-      <c r="B8">
-        <v>1.0500000000000001E-2</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
-        <v>16.2</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>33.126293995859214</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="1"/>
-        <v>1.2075</v>
-      </c>
-      <c r="G8">
-        <v>3.911282814454551E-3</v>
-      </c>
-      <c r="H8">
-        <v>9.166666666666665E-3</v>
-      </c>
-      <c r="I8">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J8">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8">
-        <v>13.6</v>
-      </c>
-      <c r="M8">
-        <v>10.3</v>
-      </c>
-      <c r="N8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>4.7</v>
-      </c>
-      <c r="B9">
-        <v>1.6799999999999999E-2</v>
-      </c>
-      <c r="C9">
-        <v>8.5</v>
-      </c>
-      <c r="D9">
-        <v>15.2</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>28.655963664238076</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="1"/>
-        <v>1.3958699999999999</v>
-      </c>
-      <c r="G9">
-        <v>4.4614194693495309E-3</v>
-      </c>
-      <c r="H9">
-        <v>1.1170528817587641E-2</v>
-      </c>
-      <c r="I9">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J9">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K9" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9">
-        <v>13.6</v>
-      </c>
-      <c r="M9">
-        <v>10.3</v>
-      </c>
-      <c r="N9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>5.6</v>
-      </c>
-      <c r="B10">
-        <v>1.9800000000000002E-2</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>14.1</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>27.448397013614407</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="1"/>
-        <v>1.4572799999999999</v>
-      </c>
-      <c r="G10">
-        <v>4.4505622402651454E-3</v>
-      </c>
-      <c r="H10">
-        <v>1.1013432454225421E-2</v>
-      </c>
-      <c r="I10">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J10">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K10" t="s">
-        <v>11</v>
-      </c>
-      <c r="L10">
-        <v>13.6</v>
-      </c>
-      <c r="M10">
-        <v>10.3</v>
-      </c>
-      <c r="N10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>6.8</v>
-      </c>
-      <c r="B11">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="C11">
-        <v>7.5</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="0"/>
-        <v>28.107158541941157</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="1"/>
-        <v>1.4231249999999998</v>
-      </c>
-      <c r="G11">
-        <v>4.6925148802466569E-3</v>
-      </c>
-      <c r="H11">
-        <v>1.3959026152646055E-2</v>
-      </c>
-      <c r="I11">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J11">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K11" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11">
-        <v>13.6</v>
-      </c>
-      <c r="M11">
-        <v>10.3</v>
-      </c>
-      <c r="N11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="B12">
-        <v>2.4E-2</v>
-      </c>
-      <c r="C12">
-        <v>7.6</v>
-      </c>
-      <c r="D12">
-        <v>9</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="0"/>
-        <v>25.091332450118433</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" si="1"/>
-        <v>1.5941759999999998</v>
-      </c>
-      <c r="G12">
-        <v>4.6035237082785061E-3</v>
-      </c>
-      <c r="H12">
-        <v>1.4920348990601998E-2</v>
-      </c>
-      <c r="I12">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J12">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K12" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12">
-        <v>13.6</v>
-      </c>
-      <c r="M12">
-        <v>10.3</v>
-      </c>
-      <c r="N12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>2.7E-2</v>
-      </c>
-      <c r="C13">
-        <v>7.5</v>
-      </c>
-      <c r="D13">
-        <v>8.6</v>
-      </c>
-      <c r="E13" s="2">
-        <f t="shared" si="0"/>
-        <v>22.902129182322419</v>
-      </c>
-      <c r="F13" s="1">
-        <f t="shared" si="1"/>
-        <v>1.7465625</v>
-      </c>
-      <c r="G13">
-        <v>4.1664368901409548E-3</v>
-      </c>
-      <c r="H13">
-        <v>1.7113031573543252E-2</v>
-      </c>
-      <c r="I13">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J13">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K13" t="s">
-        <v>11</v>
-      </c>
-      <c r="L13">
-        <v>13.6</v>
-      </c>
-      <c r="M13">
-        <v>10.3</v>
-      </c>
-      <c r="N13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>22</v>
-      </c>
-      <c r="B14">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>6.2</v>
-      </c>
-      <c r="E14" s="2">
-        <f t="shared" si="0"/>
-        <v>23.581429624170969</v>
-      </c>
-      <c r="F14" s="1">
-        <f t="shared" si="1"/>
-        <v>1.6962499999999998</v>
-      </c>
-      <c r="G14">
-        <v>4.4269179040928716E-3</v>
-      </c>
-      <c r="H14">
-        <v>2.0077633516262881E-2</v>
-      </c>
-      <c r="I14">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J14">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L14">
-        <v>13.6</v>
-      </c>
-      <c r="M14">
-        <v>10.3</v>
-      </c>
-      <c r="N14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>33</v>
-      </c>
-      <c r="B15">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="C15">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="D15">
-        <v>5.5</v>
-      </c>
-      <c r="E15" s="2">
-        <f t="shared" si="0"/>
-        <v>21.388361309309921</v>
-      </c>
-      <c r="F15" s="1">
-        <f t="shared" si="1"/>
-        <v>1.8701760000000003</v>
-      </c>
-      <c r="G15">
-        <v>4.4397430223775299E-3</v>
-      </c>
-      <c r="H15">
-        <v>2.4753867791842476E-2</v>
-      </c>
-      <c r="I15">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J15">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L15">
-        <v>13.6</v>
-      </c>
-      <c r="M15">
-        <v>10.3</v>
-      </c>
-      <c r="N15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>47</v>
-      </c>
-      <c r="B16">
-        <v>0.129</v>
-      </c>
-      <c r="C16">
-        <v>3.3</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16" s="2">
-        <f t="shared" si="0"/>
-        <v>24.759653401991859</v>
-      </c>
-      <c r="F16" s="1">
-        <f t="shared" si="1"/>
-        <v>1.6155314999999997</v>
-      </c>
-      <c r="G16">
-        <v>4.0913696062391822E-3</v>
-      </c>
-      <c r="H16">
-        <v>3.0971665618635551E-2</v>
-      </c>
-      <c r="I16">
-        <v>1.0280380382624399</v>
-      </c>
-      <c r="J16">
-        <v>2.51785650480713</v>
-      </c>
-      <c r="K16" t="s">
-        <v>11</v>
-      </c>
-      <c r="L16">
-        <v>13.6</v>
-      </c>
-      <c r="M16">
-        <v>10.3</v>
-      </c>
-      <c r="N16">
         <v>4</v>
       </c>
     </row>
@@ -3270,7 +2651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07A19C39-A8AF-48EA-8DDB-56678885135F}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
@@ -3373,6 +2754,1410 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{059866CC-3168-4352-A7B2-396C26867B98}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.47</v>
+      </c>
+      <c r="B2">
+        <v>2.8E-3</v>
+      </c>
+      <c r="C2">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <f>40/F2</f>
+        <v>28.168617343417701</v>
+      </c>
+      <c r="F2">
+        <f>C2^2*B2*1.15</f>
+        <v>1.4200199999999998</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="H2">
+        <v>5.47E-3</v>
+      </c>
+      <c r="I2">
+        <v>1.101</v>
+      </c>
+      <c r="J2">
+        <v>2.2490000000000001</v>
+      </c>
+      <c r="K2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2">
+        <v>9.6</v>
+      </c>
+      <c r="M2">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4084553-0357-4668-80B7-A59E449DE9A2}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.47</v>
+      </c>
+      <c r="B2">
+        <v>1.48E-3</v>
+      </c>
+      <c r="C2">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>42</v>
+      </c>
+      <c r="F2">
+        <f>C2^2*B2*1.15</f>
+        <v>1.2407579999999998</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3.1599999999999998E-4</v>
+      </c>
+      <c r="H2">
+        <v>4.0299999999999997E-3</v>
+      </c>
+      <c r="I2">
+        <v>1.101</v>
+      </c>
+      <c r="J2">
+        <v>2.2490000000000001</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2">
+        <v>13.6</v>
+      </c>
+      <c r="M2">
+        <v>10.3</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="C3">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="F3">
+        <f>C3^2*B3*1.15</f>
+        <v>1.163225</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3.1500000000000001E-4</v>
+      </c>
+      <c r="H3">
+        <v>6.1900000000000002E-3</v>
+      </c>
+      <c r="I3">
+        <v>1.101</v>
+      </c>
+      <c r="J3">
+        <v>2.2490000000000001</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3">
+        <v>13.6</v>
+      </c>
+      <c r="M3">
+        <v>10.3</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE769611-9C4A-4D12-ACD1-572EFA17A665}">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.45</v>
+      </c>
+      <c r="B2">
+        <v>1E-3</v>
+      </c>
+      <c r="C2">
+        <v>35</v>
+      </c>
+      <c r="D2">
+        <v>48</v>
+      </c>
+      <c r="E2" s="2">
+        <f>40/F2</f>
+        <v>28.393966282165042</v>
+      </c>
+      <c r="F2" s="5">
+        <f>C2^2*B2*1.15</f>
+        <v>1.4087499999999999</v>
+      </c>
+      <c r="G2" s="3">
+        <v>4.4930000000000002E-4</v>
+      </c>
+      <c r="H2">
+        <v>3.1449999999999998E-3</v>
+      </c>
+      <c r="I2">
+        <v>1.101</v>
+      </c>
+      <c r="J2">
+        <v>2.2490000000000001</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2">
+        <v>13.6</v>
+      </c>
+      <c r="M2">
+        <v>10.3</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.68</v>
+      </c>
+      <c r="B3">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="C3">
+        <v>31</v>
+      </c>
+      <c r="D3">
+        <v>34</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E4" si="0">40/F3</f>
+        <v>22.62136361579876</v>
+      </c>
+      <c r="F3" s="5">
+        <f t="shared" ref="F3:F4" si="1">C3^2*B3*1.15</f>
+        <v>1.76824</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3.9599999999999998E-4</v>
+      </c>
+      <c r="H3">
+        <v>4.5100000000000001E-3</v>
+      </c>
+      <c r="I3">
+        <v>1.101</v>
+      </c>
+      <c r="J3">
+        <v>2.2490000000000001</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3">
+        <v>13.6</v>
+      </c>
+      <c r="M3">
+        <v>10.3</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2.3E-3</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>24.196597353497165</v>
+      </c>
+      <c r="F4" s="5">
+        <f t="shared" si="1"/>
+        <v>1.653125</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3.9899999999999999E-4</v>
+      </c>
+      <c r="H4">
+        <v>5.1500000000000001E-3</v>
+      </c>
+      <c r="I4">
+        <v>1.101</v>
+      </c>
+      <c r="J4">
+        <v>2.2490000000000001</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4">
+        <v>13.6</v>
+      </c>
+      <c r="M4">
+        <v>10.3</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04542642-2AB9-4E4E-BC92-700C7AD35014}">
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:N1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0.36</v>
+      </c>
+      <c r="B2">
+        <v>1.0499999999999999E-3</v>
+      </c>
+      <c r="C2">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>51</v>
+      </c>
+      <c r="E2" s="2">
+        <f>40/F2</f>
+        <v>30.419002751018571</v>
+      </c>
+      <c r="F2" s="1">
+        <f>C2^2*B2*1.15</f>
+        <v>1.3149674999999996</v>
+      </c>
+      <c r="G2">
+        <v>4.4962287207989402E-3</v>
+      </c>
+      <c r="H2">
+        <v>2.7906976744186043E-3</v>
+      </c>
+      <c r="I2">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J2">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>13.6</v>
+      </c>
+      <c r="M2">
+        <v>10.3</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0.47</v>
+      </c>
+      <c r="B3">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="C3">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>46</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E16" si="0">40/F3</f>
+        <v>26.128762541806022</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F16" si="1">C3^2*B3*1.15</f>
+        <v>1.5308799999999998</v>
+      </c>
+      <c r="G3">
+        <v>4.0935840852075502E-3</v>
+      </c>
+      <c r="H3">
+        <v>3.5619552860932172E-3</v>
+      </c>
+      <c r="I3">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J3">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3">
+        <v>13.6</v>
+      </c>
+      <c r="M3">
+        <v>10.3</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B4">
+        <v>1.5900000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>33.5</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>35.001367240907847</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1428125</v>
+      </c>
+      <c r="G4">
+        <v>4.50692554059053E-3</v>
+      </c>
+      <c r="H4">
+        <v>3.695150115473441E-3</v>
+      </c>
+      <c r="I4">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J4">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4">
+        <v>13.6</v>
+      </c>
+      <c r="M4">
+        <v>10.3</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2.8500000000000001E-3</v>
+      </c>
+      <c r="C5">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>33.807268985422731</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1831775</v>
+      </c>
+      <c r="G5">
+        <v>4.2248688117616879E-3</v>
+      </c>
+      <c r="H5">
+        <v>5.4815545688757326E-3</v>
+      </c>
+      <c r="I5">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J5">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5">
+        <v>13.6</v>
+      </c>
+      <c r="M5">
+        <v>10.3</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1.5</v>
+      </c>
+      <c r="B6">
+        <v>3.8E-3</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>22</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>35.755148741418765</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1187199999999999</v>
+      </c>
+      <c r="G6">
+        <v>3.9161453990648959E-3</v>
+      </c>
+      <c r="H6">
+        <v>6.4811614241272048E-3</v>
+      </c>
+      <c r="I6">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J6">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6">
+        <v>13.6</v>
+      </c>
+      <c r="M6">
+        <v>10.3</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B7">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>40.257648953301128</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.99359999999999993</v>
+      </c>
+      <c r="G7">
+        <v>3.9723160813784969E-3</v>
+      </c>
+      <c r="H7">
+        <v>8.175399479747306E-3</v>
+      </c>
+      <c r="I7">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J7">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <v>13.6</v>
+      </c>
+      <c r="M7">
+        <v>10.3</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>3.3</v>
+      </c>
+      <c r="B8">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>16.2</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>33.126293995859214</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2075</v>
+      </c>
+      <c r="G8">
+        <v>3.911282814454551E-3</v>
+      </c>
+      <c r="H8">
+        <v>9.166666666666665E-3</v>
+      </c>
+      <c r="I8">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J8">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8">
+        <v>13.6</v>
+      </c>
+      <c r="M8">
+        <v>10.3</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4.7</v>
+      </c>
+      <c r="B9">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="C9">
+        <v>8.5</v>
+      </c>
+      <c r="D9">
+        <v>15.2</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>28.655963664238076</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3958699999999999</v>
+      </c>
+      <c r="G9">
+        <v>4.4614194693495309E-3</v>
+      </c>
+      <c r="H9">
+        <v>1.1170528817587641E-2</v>
+      </c>
+      <c r="I9">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J9">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9">
+        <v>13.6</v>
+      </c>
+      <c r="M9">
+        <v>10.3</v>
+      </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>5.6</v>
+      </c>
+      <c r="B10">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>14.1</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>27.448397013614407</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4572799999999999</v>
+      </c>
+      <c r="G10">
+        <v>4.4505622402651454E-3</v>
+      </c>
+      <c r="H10">
+        <v>1.1013432454225421E-2</v>
+      </c>
+      <c r="I10">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J10">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10">
+        <v>13.6</v>
+      </c>
+      <c r="M10">
+        <v>10.3</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>6.8</v>
+      </c>
+      <c r="B11">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="C11">
+        <v>7.5</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>28.107158541941157</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4231249999999998</v>
+      </c>
+      <c r="G11">
+        <v>4.6925148802466569E-3</v>
+      </c>
+      <c r="H11">
+        <v>1.3959026152646055E-2</v>
+      </c>
+      <c r="I11">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J11">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11">
+        <v>13.6</v>
+      </c>
+      <c r="M11">
+        <v>10.3</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B12">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C12">
+        <v>7.6</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>25.091332450118433</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5941759999999998</v>
+      </c>
+      <c r="G12">
+        <v>4.6035237082785061E-3</v>
+      </c>
+      <c r="H12">
+        <v>1.4920348990601998E-2</v>
+      </c>
+      <c r="I12">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J12">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K12" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <v>13.6</v>
+      </c>
+      <c r="M12">
+        <v>10.3</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C13">
+        <v>7.5</v>
+      </c>
+      <c r="D13">
+        <v>8.6</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>22.902129182322419</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7465625</v>
+      </c>
+      <c r="G13">
+        <v>4.1664368901409548E-3</v>
+      </c>
+      <c r="H13">
+        <v>1.7113031573543252E-2</v>
+      </c>
+      <c r="I13">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J13">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13">
+        <v>13.6</v>
+      </c>
+      <c r="M13">
+        <v>10.3</v>
+      </c>
+      <c r="N13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>6.2</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>23.581429624170969</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6962499999999998</v>
+      </c>
+      <c r="G14">
+        <v>4.4269179040928716E-3</v>
+      </c>
+      <c r="H14">
+        <v>2.0077633516262881E-2</v>
+      </c>
+      <c r="I14">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J14">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14">
+        <v>13.6</v>
+      </c>
+      <c r="M14">
+        <v>10.3</v>
+      </c>
+      <c r="N14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="C15">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D15">
+        <v>5.5</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>21.388361309309921</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8701760000000003</v>
+      </c>
+      <c r="G15">
+        <v>4.4397430223775299E-3</v>
+      </c>
+      <c r="H15">
+        <v>2.4753867791842476E-2</v>
+      </c>
+      <c r="I15">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J15">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15">
+        <v>13.6</v>
+      </c>
+      <c r="M15">
+        <v>10.3</v>
+      </c>
+      <c r="N15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>47</v>
+      </c>
+      <c r="B16">
+        <v>0.129</v>
+      </c>
+      <c r="C16">
+        <v>3.3</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>24.759653401991859</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6155314999999997</v>
+      </c>
+      <c r="G16">
+        <v>4.0913696062391822E-3</v>
+      </c>
+      <c r="H16">
+        <v>3.0971665618635551E-2</v>
+      </c>
+      <c r="I16">
+        <v>1.0280380382624399</v>
+      </c>
+      <c r="J16">
+        <v>2.51785650480713</v>
+      </c>
+      <c r="K16" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16">
+        <v>13.6</v>
+      </c>
+      <c r="M16">
+        <v>10.3</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2190A832-EF70-43A1-B39D-AE9C42882809}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="C2">
+        <v>25.5</v>
+      </c>
+      <c r="D2">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2">
+        <f>40/F2</f>
+        <v>24.314150987838367</v>
+      </c>
+      <c r="F2" s="5">
+        <f>C2^2*B2*1.15</f>
+        <v>1.6451324999999999</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5.1800000000000001E-4</v>
+      </c>
+      <c r="H2">
+        <v>4.2700000000000004E-3</v>
+      </c>
+      <c r="I2">
+        <v>1.101</v>
+      </c>
+      <c r="J2">
+        <v>2.2490000000000001</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2">
+        <v>13.6</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE43545-A402-4460-BE10-D9DDD354CCCC}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B2">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>36</v>
+      </c>
+      <c r="E2">
+        <f>40/F2</f>
+        <v>19.323671497584542</v>
+      </c>
+      <c r="F2">
+        <f>C2^2*B2*1.15</f>
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3.81E-3</v>
+      </c>
+      <c r="H2">
+        <v>5.0400000000000002E-3</v>
+      </c>
+      <c r="I2">
+        <v>1.0109999999999999</v>
+      </c>
+      <c r="J2">
+        <v>2.363</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2">
+        <v>14.5</v>
+      </c>
+      <c r="M2">
+        <v>12.8</v>
+      </c>
+      <c r="N2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>